<commit_message>
Added code to create a an excel file with the headers to extract four features for each color
</commit_message>
<xml_diff>
--- a/Binary/potato_features.xlsx
+++ b/Binary/potato_features.xlsx
@@ -14,18 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Variance</t>
-  </si>
-  <si>
-    <t>Std</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Red_Mean</t>
+  </si>
+  <si>
+    <t>Red_Median</t>
+  </si>
+  <si>
+    <t>Red_Variance</t>
+  </si>
+  <si>
+    <t>Red_Std</t>
+  </si>
+  <si>
+    <t>Green_Mean</t>
+  </si>
+  <si>
+    <t>Green_Median</t>
+  </si>
+  <si>
+    <t>Green_Variance</t>
+  </si>
+  <si>
+    <t>Green_Std</t>
+  </si>
+  <si>
+    <t>Blue_Mean</t>
+  </si>
+  <si>
+    <t>Blue_Median</t>
+  </si>
+  <si>
+    <t>Blue_Variance</t>
+  </si>
+  <si>
+    <t>Blue_Std</t>
   </si>
 </sst>
 </file>
@@ -357,13 +381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,6 +399,30 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>